<commit_message>
Added company website scraping for emails
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Shop Name</t>
   </si>
   <si>
     <t xml:space="preserve">Shop Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop Email</t>
   </si>
 </sst>
 </file>
@@ -40,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,10 +125,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -139,6 +143,9 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>